<commit_message>
AKV fertiggestellt, einheitlich alles formatiert
</commit_message>
<xml_diff>
--- a/AKV Tabelle.xlsx
+++ b/AKV Tabelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOBI\Desktop\GourmetGuide\GourmetGuide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03HornT62\bitbucket\GourmetGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0793A3A6-6306-4043-8AC7-C5AE5216EBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E29E32B-149B-44D8-BBF9-D814154414D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Aufgaben</t>
   </si>
@@ -54,41 +54,59 @@
     <t>Josi</t>
   </si>
   <si>
-    <t>Projektleiter</t>
-  </si>
-  <si>
-    <t>Backendentwickler</t>
-  </si>
-  <si>
-    <t>Frontendentwickler</t>
-  </si>
-  <si>
-    <t>Einhaltung der Projektziele</t>
-  </si>
-  <si>
-    <t>Umsetzung der UI, Benuterfreundlichkeit</t>
-  </si>
-  <si>
-    <t>Entscheidungen über Design</t>
-  </si>
-  <si>
-    <t>Funktionalität das Backends</t>
-  </si>
-  <si>
-    <t>Entwicklung der Backend Logik</t>
-  </si>
-  <si>
-    <t>Projektplanung und Steuerung, Koordination des Teams</t>
-  </si>
-  <si>
-    <t>Entscheidung über Prioritäten und Resourcen</t>
+    <t>Projektleiter, Server/- Datenbankadmin</t>
+  </si>
+  <si>
+    <t>Frontendentwickler, UI und UX Designer</t>
+  </si>
+  <si>
+    <t>Backendentwickler und Integrator</t>
+  </si>
+  <si>
+    <t>Einhaltung der Projektziele; Sicherstellung der fristgerechten Fertigstellung; Funktionsfähigkeit von Datenbank und Server</t>
+  </si>
+  <si>
+    <t>Entscheidung über Prioritäten und Projektresourcen; Zugriff auf Datenbank und Server</t>
+  </si>
+  <si>
+    <t>Projektplanung und Steuerung; Koordination des Teams; Wartung und Verwaltung der Datenbank und des Servers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sicherstellen, dass alle Features wie vorgesehen funktionieren; Dokumentieren der Testergebnisse </t>
+  </si>
+  <si>
+    <t>Zugriff auf alle zu testenden Systeme; Zuordnung von Bugfixes</t>
+  </si>
+  <si>
+    <t>Planung und Durchführung von Tests; Dokumentation von Tests</t>
+  </si>
+  <si>
+    <t>Umsetzung der UI, Benuterfreundlichkeit, Einheitlichkeit der Benutzeroberfläche</t>
+  </si>
+  <si>
+    <t>Entscheidungen über Design und Layout</t>
+  </si>
+  <si>
+    <t>Design und Umsetzung der Benutzeroberfläche; Entwicklungs des Frontends; Sicherstellen qualitative User Experience (UX)</t>
+  </si>
+  <si>
+    <t>Zugriff auf Datenbank und Serverschnittstellen</t>
+  </si>
+  <si>
+    <t>Entwicklung der Backend Logik; Integration von Frontend und Backend; API Verwaltung</t>
+  </si>
+  <si>
+    <t>Funktionalität das Backends; Stabilität und Sicherheit des Backends; Nahtlose Integration von Frontend und Backend</t>
+  </si>
+  <si>
+    <t>Funktionalitätstester</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,8 +114,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +132,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -123,13 +160,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -415,15 +458,19 @@
   <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="6" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6328125" customWidth="1"/>
+    <col min="5" max="5" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -440,7 +487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="58" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -448,52 +495,64 @@
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>13</v>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>